<commit_message>
Prise en compte des champs vides
</commit_message>
<xml_diff>
--- a/People.xlsx
+++ b/People.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samba\Documents\projects\Medical-doc-Powershell\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4145FDA3-2695-4630-B541-C2EF6D93FDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="4180" yWindow="4180" windowWidth="21600" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="main"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="152">
   <si>
     <t>firstName</t>
   </si>
@@ -133,9 +139,6 @@
     <t>Labbati</t>
   </si>
   <si>
-    <t>Genderqueer</t>
-  </si>
-  <si>
     <t>Viva</t>
   </si>
   <si>
@@ -214,9 +217,6 @@
     <t>Mountlow</t>
   </si>
   <si>
-    <t>Genderfluid</t>
-  </si>
-  <si>
     <t>Mynte</t>
   </si>
   <si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>Dolbey</t>
-  </si>
-  <si>
-    <t>Agender</t>
   </si>
   <si>
     <t>Twinte</t>
@@ -484,7 +481,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -535,16 +532,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFbfbfbf"/>
+        <color rgb="FFBFBFBF"/>
       </left>
       <right style="thin">
-        <color rgb="FFbfbfbf"/>
+        <color rgb="FFBFBFBF"/>
       </right>
       <top style="thin">
-        <color rgb="FFbfbfbf"/>
+        <color rgb="FFBFBFBF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFbfbfbf"/>
+        <color rgb="FFBFBFBF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,40 +550,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -597,10 +593,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -638,71 +634,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -730,7 +726,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -753,11 +749,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -766,13 +762,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -782,7 +778,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -791,7 +787,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -800,7 +796,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -808,10 +804,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -876,45 +872,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="12.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="12.453125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +928,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -990,7 +966,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1004,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1066,7 +1042,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1104,7 +1080,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1142,7 +1118,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1180,7 +1156,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1218,7 +1194,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1256,7 +1232,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1294,7 +1270,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1332,7 +1308,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1343,10 +1319,10 @@
         <v>26386</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1370,12 +1346,12 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C13" s="4">
         <v>37121</v>
@@ -1384,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1408,12 +1384,12 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C14" s="4">
         <v>34478</v>
@@ -1422,7 +1398,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1446,12 +1422,12 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C15" s="4">
         <v>34480</v>
@@ -1484,12 +1460,12 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C16" s="4">
         <v>34405</v>
@@ -1498,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1522,12 +1498,12 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C17" s="4">
         <v>30164</v>
@@ -1536,7 +1512,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1560,12 +1536,12 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row r="18" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="4">
         <v>36368</v>
@@ -1574,7 +1550,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1598,12 +1574,12 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row r="19" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C19" s="4">
         <v>36776</v>
@@ -1612,7 +1588,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1636,12 +1612,12 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row r="20" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="C20" s="4">
         <v>36741</v>
@@ -1650,7 +1626,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1674,21 +1650,21 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C21" s="4">
         <v>35498</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1712,12 +1688,12 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4">
         <v>30040</v>
@@ -1726,7 +1702,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1750,12 +1726,12 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="4">
         <v>32361</v>
@@ -1764,7 +1740,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1788,12 +1764,12 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="4">
         <v>26154</v>
@@ -1802,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1826,12 +1802,12 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" s="4">
         <v>30566</v>
@@ -1840,7 +1816,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1864,21 +1840,21 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4">
         <v>32608</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1902,12 +1878,12 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4">
         <v>27112</v>
@@ -1916,7 +1892,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1940,12 +1916,12 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="4">
         <v>32326</v>
@@ -1954,7 +1930,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1978,21 +1954,21 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="4">
         <v>33426</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2016,12 +1992,12 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" s="4">
         <v>33466</v>
@@ -2030,7 +2006,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2054,12 +2030,12 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" s="4">
         <v>34446</v>
@@ -2068,7 +2044,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2092,12 +2068,12 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C32" s="4">
         <v>27547</v>
@@ -2106,7 +2082,7 @@
         <v>23</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2130,12 +2106,12 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row r="33" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C33" s="4">
         <v>26426</v>
@@ -2144,7 +2120,7 @@
         <v>23</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -2168,12 +2144,12 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row r="34" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" s="4">
         <v>36246</v>
@@ -2182,7 +2158,7 @@
         <v>23</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2206,12 +2182,12 @@
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row r="35" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C35" s="4">
         <v>28404</v>
@@ -2220,7 +2196,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2244,12 +2220,12 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row r="36" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="4">
         <v>30524</v>
@@ -2282,12 +2258,12 @@
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="37" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C37" s="4">
         <v>27373</v>
@@ -2296,7 +2272,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2320,12 +2296,12 @@
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row r="38" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C38" s="4">
         <v>33698</v>
@@ -2334,7 +2310,7 @@
         <v>23</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2358,12 +2334,12 @@
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row r="39" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C39" s="4">
         <v>32770</v>
@@ -2372,7 +2348,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -2396,12 +2372,12 @@
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row r="40" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C40" s="4">
         <v>32197</v>
@@ -2410,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -2434,12 +2410,12 @@
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row r="41" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C41" s="4">
         <v>32359</v>
@@ -2448,7 +2424,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -2472,12 +2448,12 @@
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row r="42" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C42" s="4">
         <v>31715</v>
@@ -2486,7 +2462,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -2510,12 +2486,12 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row r="43" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C43" s="4">
         <v>26295</v>
@@ -2524,7 +2500,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2548,12 +2524,12 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row r="44" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C44" s="4">
         <v>27219</v>
@@ -2586,12 +2562,12 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row r="45" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C45" s="4">
         <v>35878</v>
@@ -2600,7 +2576,7 @@
         <v>7</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -2624,12 +2600,12 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row r="46" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C46" s="4">
         <v>27353</v>
@@ -2638,7 +2614,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2662,12 +2638,12 @@
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row r="47" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C47" s="4">
         <v>29959</v>
@@ -2676,7 +2652,7 @@
         <v>7</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -2700,12 +2676,12 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row r="48" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C48" s="4">
         <v>25745</v>
@@ -2714,7 +2690,7 @@
         <v>23</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2738,12 +2714,12 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row r="49" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C49" s="4">
         <v>35026</v>
@@ -2752,7 +2728,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -2776,12 +2752,12 @@
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+    <row r="50" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C50" s="4">
         <v>31451</v>
@@ -2790,7 +2766,7 @@
         <v>23</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -2814,12 +2790,12 @@
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+    <row r="51" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C51" s="4">
         <v>32284</v>
@@ -2828,7 +2804,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>

</xml_diff>